<commit_message>
biphasic detection, inverse agonist mode
</commit_message>
<xml_diff>
--- a/inst/docs/Example-Dose-Response-SEL.xlsx
+++ b/inst/docs/Example-Dose-Response-SEL.xlsx
@@ -2531,7 +2531,7 @@
         <v>20</v>
       </c>
       <c r="C41" s="18">
-        <v>95.146</v>
+        <v>80</v>
       </c>
       <c r="D41" s="4"/>
       <c r="E41" s="4"/>
@@ -2691,7 +2691,7 @@
         <v>20</v>
       </c>
       <c r="C51" s="18">
-        <v>96.233</v>
+        <v>82</v>
       </c>
       <c r="D51" s="4"/>
       <c r="E51" s="4"/>
@@ -2851,7 +2851,7 @@
         <v>20</v>
       </c>
       <c r="C61" s="18">
-        <v>95.54600000000001</v>
+        <v>79</v>
       </c>
       <c r="D61" s="4"/>
       <c r="E61" s="4"/>

</xml_diff>

<commit_message>
updating tests to include inactive curve
</commit_message>
<xml_diff>
--- a/inst/docs/Example-Dose-Response-SEL.xlsx
+++ b/inst/docs/Example-Dose-Response-SEL.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24709"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25516"/>
   <workbookPr date1904="1" autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060"/>
@@ -68,7 +68,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="51">
   <si>
     <t>Experiment Meta Data</t>
   </si>
@@ -121,9 +121,6 @@
     <t>Text</t>
   </si>
   <si>
-    <t>Number</t>
-  </si>
-  <si>
     <t>Corporate Batch ID</t>
   </si>
   <si>
@@ -131,18 +128,6 @@
   </si>
   <si>
     <t>curve id</t>
-  </si>
-  <si>
-    <t>Max (efficacy)</t>
-  </si>
-  <si>
-    <t>Min (efficacy)</t>
-  </si>
-  <si>
-    <t>EC50 (uM)</t>
-  </si>
-  <si>
-    <t>Hill slope</t>
   </si>
   <si>
     <t>Category</t>
@@ -155,9 +140,6 @@
   </si>
   <si>
     <t>a</t>
-  </si>
-  <si>
-    <t>sigmoid</t>
   </si>
   <si>
     <t>b</t>
@@ -205,9 +187,6 @@
     <t>CMPD-0000011-01A</t>
   </si>
   <si>
-    <t>biphasic</t>
-  </si>
-  <si>
     <t>Raw Results</t>
   </si>
   <si>
@@ -239,6 +218,9 @@
   </si>
   <si>
     <t>Dose Response Protocol</t>
+  </si>
+  <si>
+    <t>inactive</t>
   </si>
 </sst>
 </file>
@@ -1866,8 +1848,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:IV1360"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A48" workbookViewId="0">
+      <selection activeCell="C37" sqref="C37:C76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0"/>
@@ -1914,7 +1896,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="C3" s="4"/>
       <c r="D3" s="7"/>
@@ -1928,7 +1910,7 @@
         <v>4</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="C4" s="8"/>
       <c r="D4" s="9" t="s">
@@ -2029,489 +2011,303 @@
       <c r="C11" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="D11" s="18" t="s">
-        <v>17</v>
-      </c>
-      <c r="E11" s="18" t="s">
-        <v>17</v>
-      </c>
-      <c r="F11" s="18" t="s">
-        <v>17</v>
-      </c>
-      <c r="G11" s="18" t="s">
-        <v>17</v>
-      </c>
-      <c r="H11" s="18" t="s">
-        <v>16</v>
-      </c>
+      <c r="D11" s="4"/>
+      <c r="E11" s="4"/>
+      <c r="F11" s="4"/>
+      <c r="G11" s="4"/>
+      <c r="H11" s="4"/>
     </row>
     <row r="12" spans="1:8" ht="15" customHeight="1">
       <c r="A12" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B12" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="B12" s="11" t="s">
+      <c r="C12" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="C12" s="11" t="s">
+      <c r="D12" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="D12" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="E12" s="18" t="s">
-        <v>22</v>
-      </c>
-      <c r="F12" s="18" t="s">
-        <v>23</v>
-      </c>
-      <c r="G12" s="18" t="s">
-        <v>24</v>
-      </c>
-      <c r="H12" s="18" t="s">
-        <v>25</v>
-      </c>
+      <c r="E12" s="4"/>
+      <c r="F12" s="4"/>
+      <c r="G12" s="4"/>
+      <c r="H12" s="4"/>
     </row>
     <row r="13" spans="1:8" ht="15" customHeight="1">
       <c r="A13" s="19" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="B13" s="19" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="C13" s="19" t="s">
-        <v>28</v>
-      </c>
-      <c r="D13" s="18">
-        <v>102.911</v>
-      </c>
-      <c r="E13" s="18">
-        <v>0</v>
-      </c>
-      <c r="F13" s="18">
-        <v>0.41481459999999998</v>
-      </c>
-      <c r="G13" s="18">
-        <v>0.73779899999999998</v>
-      </c>
-      <c r="H13" s="18" t="s">
-        <v>29</v>
-      </c>
+        <v>23</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="E13" s="4"/>
+      <c r="F13" s="4"/>
+      <c r="G13" s="4"/>
+      <c r="H13" s="4"/>
     </row>
     <row r="14" spans="1:8" ht="15" customHeight="1">
       <c r="A14" s="18" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="B14" s="18" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="C14" s="18" t="s">
-        <v>30</v>
-      </c>
-      <c r="D14" s="18">
-        <v>100</v>
-      </c>
-      <c r="E14" s="18">
-        <v>0</v>
-      </c>
-      <c r="F14" s="18">
-        <v>0.52504680000000004</v>
-      </c>
-      <c r="G14" s="18">
-        <v>0.98607500000000003</v>
-      </c>
-      <c r="H14" s="18" t="s">
-        <v>29</v>
-      </c>
+        <v>24</v>
+      </c>
+      <c r="D14" s="4"/>
+      <c r="E14" s="4"/>
+      <c r="F14" s="4"/>
+      <c r="G14" s="4"/>
+      <c r="H14" s="4"/>
     </row>
     <row r="15" spans="1:8" ht="15" customHeight="1">
       <c r="A15" s="18" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="B15" s="18" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="C15" s="18" t="s">
-        <v>32</v>
-      </c>
-      <c r="D15" s="18">
-        <v>100</v>
-      </c>
-      <c r="E15" s="18">
-        <v>0</v>
-      </c>
-      <c r="F15" s="18">
-        <v>0.56237890000000001</v>
-      </c>
-      <c r="G15" s="18">
-        <v>0.64493500000000004</v>
-      </c>
-      <c r="H15" s="18" t="s">
-        <v>29</v>
-      </c>
+        <v>26</v>
+      </c>
+      <c r="D15" s="4"/>
+      <c r="E15" s="4"/>
+      <c r="F15" s="4"/>
+      <c r="G15" s="4"/>
+      <c r="H15" s="4"/>
     </row>
     <row r="16" spans="1:8" ht="15" customHeight="1">
       <c r="A16" s="18" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="B16" s="18" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="C16" s="18" t="s">
-        <v>34</v>
-      </c>
-      <c r="D16" s="18">
-        <v>100</v>
-      </c>
-      <c r="E16" s="18">
-        <v>0</v>
-      </c>
-      <c r="F16" s="18">
-        <v>0.94129750000000001</v>
-      </c>
-      <c r="G16" s="18">
-        <v>0.93187399999999998</v>
-      </c>
-      <c r="H16" s="18" t="s">
-        <v>29</v>
-      </c>
+        <v>28</v>
+      </c>
+      <c r="D16" s="4"/>
+      <c r="E16" s="4"/>
+      <c r="F16" s="4"/>
+      <c r="G16" s="4"/>
+      <c r="H16" s="4"/>
     </row>
     <row r="17" spans="1:8" ht="15" customHeight="1">
       <c r="A17" s="18" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="B17" s="18" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="C17" s="18" t="s">
-        <v>36</v>
-      </c>
-      <c r="D17" s="18">
-        <v>100</v>
-      </c>
-      <c r="E17" s="18">
-        <v>0</v>
-      </c>
-      <c r="F17" s="18">
-        <v>0.81614209999999998</v>
-      </c>
-      <c r="G17" s="18">
-        <v>0.69671300000000003</v>
-      </c>
-      <c r="H17" s="18" t="s">
-        <v>29</v>
-      </c>
+        <v>30</v>
+      </c>
+      <c r="D17" s="4"/>
+      <c r="E17" s="4"/>
+      <c r="F17" s="4"/>
+      <c r="G17" s="4"/>
+      <c r="H17" s="4"/>
     </row>
     <row r="18" spans="1:8" ht="15" customHeight="1">
       <c r="A18" s="18" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="B18" s="18" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="C18" s="18" t="s">
-        <v>38</v>
-      </c>
-      <c r="D18" s="18">
-        <v>100</v>
-      </c>
-      <c r="E18" s="18">
-        <v>0</v>
-      </c>
-      <c r="F18" s="18">
-        <v>0.5187678</v>
-      </c>
-      <c r="G18" s="18">
-        <v>0.71002399999999999</v>
-      </c>
-      <c r="H18" s="18" t="s">
-        <v>29</v>
-      </c>
+        <v>32</v>
+      </c>
+      <c r="D18" s="4"/>
+      <c r="E18" s="4"/>
+      <c r="F18" s="4"/>
+      <c r="G18" s="4"/>
+      <c r="H18" s="4"/>
     </row>
     <row r="19" spans="1:8" ht="15" customHeight="1">
       <c r="A19" s="18" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="B19" s="18" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="C19" s="18">
         <v>90803</v>
       </c>
-      <c r="D19" s="18">
-        <v>89.529600000000002</v>
-      </c>
-      <c r="E19" s="18">
-        <v>0</v>
-      </c>
-      <c r="F19" s="18">
-        <v>0.51838930000000005</v>
-      </c>
-      <c r="G19" s="18">
-        <v>1.4231799999999999</v>
-      </c>
-      <c r="H19" s="18" t="s">
-        <v>29</v>
-      </c>
+      <c r="D19" s="4"/>
+      <c r="E19" s="4"/>
+      <c r="F19" s="4"/>
+      <c r="G19" s="4"/>
+      <c r="H19" s="4"/>
     </row>
     <row r="20" spans="1:8" ht="15" customHeight="1">
       <c r="A20" s="18" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="B20" s="18" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="C20" s="18">
         <v>90816</v>
       </c>
-      <c r="D20" s="18">
-        <v>100</v>
-      </c>
-      <c r="E20" s="18">
-        <v>0</v>
-      </c>
-      <c r="F20" s="18">
-        <v>0.9263555</v>
-      </c>
-      <c r="G20" s="18">
-        <v>1.21865</v>
-      </c>
-      <c r="H20" s="18" t="s">
-        <v>29</v>
-      </c>
+      <c r="D20" s="4"/>
+      <c r="E20" s="4"/>
+      <c r="F20" s="4"/>
+      <c r="G20" s="4"/>
+      <c r="H20" s="4"/>
     </row>
     <row r="21" spans="1:8" ht="15" customHeight="1">
       <c r="A21" s="18" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="B21" s="18" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="C21" s="18">
         <v>126226</v>
       </c>
-      <c r="D21" s="18">
-        <v>100</v>
-      </c>
-      <c r="E21" s="18">
-        <v>0</v>
-      </c>
-      <c r="F21" s="18">
-        <v>1.5161180000000001</v>
-      </c>
-      <c r="G21" s="18">
-        <v>1.0336700000000001</v>
-      </c>
-      <c r="H21" s="18" t="s">
-        <v>29</v>
-      </c>
+      <c r="D21" s="4"/>
+      <c r="E21" s="4"/>
+      <c r="F21" s="4"/>
+      <c r="G21" s="4"/>
+      <c r="H21" s="4"/>
     </row>
     <row r="22" spans="1:8" ht="15" customHeight="1">
       <c r="A22" s="18" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="B22" s="18" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="C22" s="18">
         <v>126877</v>
       </c>
-      <c r="D22" s="18">
-        <v>100</v>
-      </c>
-      <c r="E22" s="18">
-        <v>0</v>
-      </c>
-      <c r="F22" s="18">
-        <v>2.1336979999999999</v>
-      </c>
-      <c r="G22" s="18">
-        <v>1.21384</v>
-      </c>
-      <c r="H22" s="18" t="s">
-        <v>29</v>
-      </c>
+      <c r="D22" s="4"/>
+      <c r="E22" s="4"/>
+      <c r="F22" s="4"/>
+      <c r="G22" s="4"/>
+      <c r="H22" s="4"/>
     </row>
     <row r="23" spans="1:8" ht="15" customHeight="1">
       <c r="A23" s="18" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="B23" s="18" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="C23" s="18">
         <v>126915</v>
       </c>
-      <c r="D23" s="18">
-        <v>100</v>
-      </c>
-      <c r="E23" s="18">
-        <v>0</v>
-      </c>
-      <c r="F23" s="18">
-        <v>1.6199330000000001</v>
-      </c>
-      <c r="G23" s="18">
-        <v>1.2856700000000001</v>
-      </c>
-      <c r="H23" s="18" t="s">
-        <v>29</v>
-      </c>
+      <c r="D23" s="4"/>
+      <c r="E23" s="4"/>
+      <c r="F23" s="4"/>
+      <c r="G23" s="4"/>
+      <c r="H23" s="4"/>
     </row>
     <row r="24" spans="1:8" ht="15" customHeight="1">
       <c r="A24" s="18" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="B24" s="18" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="C24" s="18">
         <v>126933</v>
       </c>
-      <c r="D24" s="18">
-        <v>100</v>
-      </c>
-      <c r="E24" s="18">
-        <v>0</v>
-      </c>
-      <c r="F24" s="18">
-        <v>1.1086009999999999</v>
-      </c>
-      <c r="G24" s="18">
-        <v>0.87272099999999997</v>
-      </c>
-      <c r="H24" s="18" t="s">
-        <v>29</v>
-      </c>
+      <c r="D24" s="4"/>
+      <c r="E24" s="4"/>
+      <c r="F24" s="4"/>
+      <c r="G24" s="4"/>
+      <c r="H24" s="4"/>
     </row>
     <row r="25" spans="1:8" ht="15" customHeight="1">
       <c r="A25" s="18" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="B25" s="18" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="C25" s="18">
         <v>8778</v>
       </c>
-      <c r="D25" s="18">
-        <v>100</v>
-      </c>
-      <c r="E25" s="18">
-        <v>0</v>
-      </c>
-      <c r="F25" s="18">
-        <v>0.9263555</v>
-      </c>
-      <c r="G25" s="18">
-        <v>1.21865</v>
-      </c>
-      <c r="H25" s="18" t="s">
-        <v>45</v>
-      </c>
+      <c r="D25" s="4"/>
+      <c r="E25" s="4"/>
+      <c r="F25" s="4"/>
+      <c r="G25" s="4"/>
+      <c r="H25" s="4"/>
     </row>
     <row r="26" spans="1:8" ht="15" customHeight="1">
       <c r="A26" s="18" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="B26" s="18" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="C26" s="18">
         <v>8788</v>
       </c>
-      <c r="D26" s="18">
-        <v>100</v>
-      </c>
-      <c r="E26" s="18">
-        <v>0</v>
-      </c>
-      <c r="F26" s="18">
-        <v>1.5161180000000001</v>
-      </c>
-      <c r="G26" s="18">
-        <v>1.0336700000000001</v>
-      </c>
-      <c r="H26" s="18" t="s">
-        <v>45</v>
-      </c>
+      <c r="D26" s="4"/>
+      <c r="E26" s="4"/>
+      <c r="F26" s="4"/>
+      <c r="G26" s="4"/>
+      <c r="H26" s="4"/>
     </row>
     <row r="27" spans="1:8" ht="15" customHeight="1">
       <c r="A27" s="18" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="B27" s="18" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="C27" s="18">
         <v>8806</v>
       </c>
-      <c r="D27" s="18">
-        <v>100</v>
-      </c>
-      <c r="E27" s="18">
-        <v>0</v>
-      </c>
-      <c r="F27" s="18">
-        <v>2.1336979999999999</v>
-      </c>
-      <c r="G27" s="18">
-        <v>1.21384</v>
-      </c>
-      <c r="H27" s="18" t="s">
-        <v>45</v>
-      </c>
+      <c r="D27" s="4"/>
+      <c r="E27" s="4"/>
+      <c r="F27" s="4"/>
+      <c r="G27" s="4"/>
+      <c r="H27" s="4"/>
     </row>
     <row r="28" spans="1:8" ht="15" customHeight="1">
       <c r="A28" s="18" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="B28" s="18" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="C28" s="18">
         <v>8836</v>
       </c>
-      <c r="D28" s="18">
-        <v>100</v>
-      </c>
-      <c r="E28" s="18">
-        <v>0</v>
-      </c>
-      <c r="F28" s="18">
-        <v>1.6199330000000001</v>
-      </c>
-      <c r="G28" s="18">
-        <v>1.2856700000000001</v>
-      </c>
-      <c r="H28" s="18" t="s">
-        <v>45</v>
-      </c>
+      <c r="D28" s="4"/>
+      <c r="E28" s="4"/>
+      <c r="F28" s="4"/>
+      <c r="G28" s="4"/>
+      <c r="H28" s="4"/>
     </row>
     <row r="29" spans="1:8" ht="15" customHeight="1">
       <c r="A29" s="18" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="B29" s="18" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="C29" s="18">
         <v>9629</v>
       </c>
-      <c r="D29" s="18">
-        <v>100</v>
-      </c>
-      <c r="E29" s="18">
-        <v>0</v>
-      </c>
-      <c r="F29" s="18">
-        <v>1.1086009999999999</v>
-      </c>
-      <c r="G29" s="18">
-        <v>0.87272099999999997</v>
-      </c>
-      <c r="H29" s="18" t="s">
-        <v>45</v>
-      </c>
+      <c r="D29" s="4"/>
+      <c r="E29" s="4"/>
+      <c r="F29" s="4"/>
+      <c r="G29" s="4"/>
+      <c r="H29" s="4"/>
     </row>
     <row r="30" spans="1:8" ht="15" customHeight="1">
       <c r="A30" s="4"/>
@@ -2555,7 +2351,7 @@
     </row>
     <row r="34" spans="1:8" ht="15" customHeight="1">
       <c r="A34" s="20" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="B34" s="21"/>
       <c r="C34" s="7"/>
@@ -2567,16 +2363,16 @@
     </row>
     <row r="35" spans="1:8" ht="15" customHeight="1">
       <c r="A35" s="22" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="B35" s="11" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="C35" s="11" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="D35" s="11" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="E35" s="3"/>
       <c r="F35" s="4"/>
@@ -2585,16 +2381,16 @@
     </row>
     <row r="36" spans="1:8" ht="15" customHeight="1">
       <c r="A36" s="19" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B36" s="19" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="C36" s="19" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="D36" s="19" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="E36" s="4"/>
       <c r="F36" s="4"/>
@@ -2603,13 +2399,13 @@
     </row>
     <row r="37" spans="1:8" ht="15" customHeight="1">
       <c r="A37" s="18" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="B37" s="18">
         <v>20</v>
       </c>
       <c r="C37" s="18">
-        <v>88.51</v>
+        <v>3.1563188985455799</v>
       </c>
       <c r="D37" s="4"/>
       <c r="E37" s="4"/>
@@ -2619,16 +2415,16 @@
     </row>
     <row r="38" spans="1:8" ht="15" customHeight="1">
       <c r="A38" s="18" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="B38" s="18">
         <v>10</v>
       </c>
       <c r="C38" s="18">
-        <v>89.825999999999993</v>
+        <v>9.4678847573231906</v>
       </c>
       <c r="D38" s="18" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="E38" s="4"/>
       <c r="F38" s="4"/>
@@ -2637,13 +2433,13 @@
     </row>
     <row r="39" spans="1:8" ht="15" customHeight="1">
       <c r="A39" s="18" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="B39" s="18">
         <v>5</v>
       </c>
       <c r="C39" s="18">
-        <v>89.882999999999996</v>
+        <v>5.7637254113797098</v>
       </c>
       <c r="D39" s="4"/>
       <c r="E39" s="4"/>
@@ -2653,13 +2449,13 @@
     </row>
     <row r="40" spans="1:8" ht="15" customHeight="1">
       <c r="A40" s="18" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="B40" s="18">
         <v>2.5</v>
       </c>
       <c r="C40" s="18">
-        <v>79.299000000000007</v>
+        <v>9.0924222476314807</v>
       </c>
       <c r="D40" s="4"/>
       <c r="E40" s="4"/>
@@ -2669,13 +2465,13 @@
     </row>
     <row r="41" spans="1:8" ht="15" customHeight="1">
       <c r="A41" s="18" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="B41" s="18">
         <v>1.25</v>
       </c>
       <c r="C41" s="18">
-        <v>67.286000000000001</v>
+        <v>17.008430556161301</v>
       </c>
       <c r="D41" s="4"/>
       <c r="E41" s="4"/>
@@ -2685,13 +2481,13 @@
     </row>
     <row r="42" spans="1:8" ht="15" customHeight="1">
       <c r="A42" s="18" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="B42" s="18">
         <v>0.625</v>
       </c>
       <c r="C42" s="18">
-        <v>44.002000000000002</v>
+        <v>0.98230094765313003</v>
       </c>
       <c r="D42" s="4"/>
       <c r="E42" s="4"/>
@@ -2701,13 +2497,13 @@
     </row>
     <row r="43" spans="1:8" ht="15" customHeight="1">
       <c r="A43" s="18" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="B43" s="18">
         <v>0.3125</v>
       </c>
       <c r="C43" s="18">
-        <v>38.853000000000002</v>
+        <v>-3.0684522946830799</v>
       </c>
       <c r="D43" s="4"/>
       <c r="E43" s="4"/>
@@ -2717,13 +2513,13 @@
     </row>
     <row r="44" spans="1:8" ht="15" customHeight="1">
       <c r="A44" s="18" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="B44" s="18">
         <v>0.15625</v>
       </c>
       <c r="C44" s="18">
-        <v>23.75</v>
+        <v>13.357313459273399</v>
       </c>
       <c r="D44" s="4"/>
       <c r="E44" s="4"/>
@@ -2733,13 +2529,13 @@
     </row>
     <row r="45" spans="1:8" ht="15" customHeight="1">
       <c r="A45" s="18" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="B45" s="18">
         <v>7.8125E-2</v>
       </c>
       <c r="C45" s="18">
-        <v>32.331000000000003</v>
+        <v>-2.9221484391018699</v>
       </c>
       <c r="D45" s="4"/>
       <c r="E45" s="4"/>
@@ -2749,13 +2545,13 @@
     </row>
     <row r="46" spans="1:8" ht="15" customHeight="1">
       <c r="A46" s="18" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="B46" s="18">
         <v>3.9063000000000001E-2</v>
       </c>
       <c r="C46" s="18">
-        <v>11.565</v>
+        <v>3.96152534405701</v>
       </c>
       <c r="D46" s="4"/>
       <c r="E46" s="4"/>
@@ -2765,13 +2561,13 @@
     </row>
     <row r="47" spans="1:8" ht="15" customHeight="1">
       <c r="A47" s="18" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="B47" s="18">
         <v>20</v>
       </c>
       <c r="C47" s="18">
-        <v>80</v>
+        <v>-2.2800829273182899</v>
       </c>
       <c r="D47" s="4"/>
       <c r="E47" s="4"/>
@@ -2781,13 +2577,13 @@
     </row>
     <row r="48" spans="1:8" ht="15" customHeight="1">
       <c r="A48" s="18" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="B48" s="18">
         <v>10</v>
       </c>
       <c r="C48" s="18">
-        <v>95.546000000000006</v>
+        <v>2.68060458358377</v>
       </c>
       <c r="D48" s="4"/>
       <c r="E48" s="4"/>
@@ -2797,13 +2593,13 @@
     </row>
     <row r="49" spans="1:8" ht="15" customHeight="1">
       <c r="A49" s="18" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="B49" s="18">
         <v>5</v>
       </c>
       <c r="C49" s="18">
-        <v>92.742999999999995</v>
+        <v>12.9902945121285</v>
       </c>
       <c r="D49" s="4"/>
       <c r="E49" s="4"/>
@@ -2813,13 +2609,13 @@
     </row>
     <row r="50" spans="1:8" ht="15" customHeight="1">
       <c r="A50" s="18" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="B50" s="18">
         <v>2.5</v>
       </c>
       <c r="C50" s="18">
-        <v>89.54</v>
+        <v>0.65227452316321399</v>
       </c>
       <c r="D50" s="4"/>
       <c r="E50" s="4"/>
@@ -2829,13 +2625,13 @@
     </row>
     <row r="51" spans="1:8" ht="15" customHeight="1">
       <c r="A51" s="18" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="B51" s="18">
         <v>1.25</v>
       </c>
       <c r="C51" s="18">
-        <v>71.805000000000007</v>
+        <v>8.5978110367432201</v>
       </c>
       <c r="D51" s="4"/>
       <c r="E51" s="4"/>
@@ -2845,13 +2641,13 @@
     </row>
     <row r="52" spans="1:8" ht="15" customHeight="1">
       <c r="A52" s="18" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="B52" s="18">
         <v>0.625</v>
       </c>
       <c r="C52" s="18">
-        <v>60.993000000000002</v>
+        <v>13.039797001984001</v>
       </c>
       <c r="D52" s="4"/>
       <c r="E52" s="4"/>
@@ -2861,13 +2657,13 @@
     </row>
     <row r="53" spans="1:8" ht="15" customHeight="1">
       <c r="A53" s="18" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="B53" s="18">
         <v>0.3125</v>
       </c>
       <c r="C53" s="18">
-        <v>49.322000000000003</v>
+        <v>1.12833725172095</v>
       </c>
       <c r="D53" s="4"/>
       <c r="E53" s="4"/>
@@ -2877,13 +2673,13 @@
     </row>
     <row r="54" spans="1:8" ht="15" customHeight="1">
       <c r="A54" s="18" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="B54" s="18">
         <v>0.15625</v>
       </c>
       <c r="C54" s="18">
-        <v>32.789000000000001</v>
+        <v>13.4905526635703</v>
       </c>
       <c r="D54" s="4"/>
       <c r="E54" s="4"/>
@@ -2893,13 +2689,13 @@
     </row>
     <row r="55" spans="1:8" ht="15" customHeight="1">
       <c r="A55" s="18" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="B55" s="18">
         <v>7.8125E-2</v>
       </c>
       <c r="C55" s="18">
-        <v>20.146000000000001</v>
+        <v>1.4143550640437801</v>
       </c>
       <c r="D55" s="4"/>
       <c r="E55" s="4"/>
@@ -2909,13 +2705,13 @@
     </row>
     <row r="56" spans="1:8" ht="15" customHeight="1">
       <c r="A56" s="18" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="B56" s="18">
         <v>3.9063000000000001E-2</v>
       </c>
       <c r="C56" s="18">
-        <v>27.353999999999999</v>
+        <v>1.18588131037541</v>
       </c>
       <c r="D56" s="4"/>
       <c r="E56" s="4"/>
@@ -2925,13 +2721,13 @@
     </row>
     <row r="57" spans="1:8" ht="15" customHeight="1">
       <c r="A57" s="18" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="B57" s="18">
         <v>20</v>
       </c>
       <c r="C57" s="18">
-        <v>82</v>
+        <v>11.456760535948</v>
       </c>
       <c r="D57" s="4"/>
       <c r="E57" s="4"/>
@@ -2941,13 +2737,13 @@
     </row>
     <row r="58" spans="1:8" ht="15" customHeight="1">
       <c r="A58" s="18" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="B58" s="18">
         <v>10</v>
       </c>
       <c r="C58" s="18">
-        <v>92.286000000000001</v>
+        <v>14.525231706211301</v>
       </c>
       <c r="D58" s="4"/>
       <c r="E58" s="4"/>
@@ -2957,13 +2753,13 @@
     </row>
     <row r="59" spans="1:8" ht="15" customHeight="1">
       <c r="A59" s="18" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="B59" s="18">
         <v>5</v>
       </c>
       <c r="C59" s="18">
-        <v>90.111999999999995</v>
+        <v>11.0169733164366</v>
       </c>
       <c r="D59" s="4"/>
       <c r="E59" s="4"/>
@@ -2973,13 +2769,13 @@
     </row>
     <row r="60" spans="1:8" ht="15" customHeight="1">
       <c r="A60" s="18" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="B60" s="18">
         <v>2.5</v>
       </c>
       <c r="C60" s="18">
-        <v>87.423000000000002</v>
+        <v>7.8644100157543999</v>
       </c>
       <c r="D60" s="4"/>
       <c r="E60" s="4"/>
@@ -2989,13 +2785,13 @@
     </row>
     <row r="61" spans="1:8" ht="15" customHeight="1">
       <c r="A61" s="18" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="B61" s="18">
         <v>1.25</v>
       </c>
       <c r="C61" s="18">
-        <v>75.924000000000007</v>
+        <v>12.8446836478543</v>
       </c>
       <c r="D61" s="4"/>
       <c r="E61" s="4"/>
@@ -3005,13 +2801,13 @@
     </row>
     <row r="62" spans="1:8" ht="15" customHeight="1">
       <c r="A62" s="18" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="B62" s="18">
         <v>0.625</v>
       </c>
       <c r="C62" s="18">
-        <v>50.581000000000003</v>
+        <v>13.590515141840999</v>
       </c>
       <c r="D62" s="4"/>
       <c r="E62" s="4"/>
@@ -3021,13 +2817,13 @@
     </row>
     <row r="63" spans="1:8" ht="15" customHeight="1">
       <c r="A63" s="18" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="B63" s="18">
         <v>0.3125</v>
       </c>
       <c r="C63" s="18">
-        <v>48.863999999999997</v>
+        <v>4.7513596469070798</v>
       </c>
       <c r="D63" s="4"/>
       <c r="E63" s="4"/>
@@ -3037,13 +2833,13 @@
     </row>
     <row r="64" spans="1:8" ht="15" customHeight="1">
       <c r="A64" s="18" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="B64" s="18">
         <v>0.15625</v>
       </c>
       <c r="C64" s="18">
-        <v>37.479999999999997</v>
+        <v>1.1087261070497301</v>
       </c>
       <c r="D64" s="4"/>
       <c r="E64" s="4"/>
@@ -3053,13 +2849,13 @@
     </row>
     <row r="65" spans="1:8" ht="15" customHeight="1">
       <c r="A65" s="18" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="B65" s="18">
         <v>7.8125E-2</v>
       </c>
       <c r="C65" s="18">
-        <v>31.015000000000001</v>
+        <v>14.013658881885901</v>
       </c>
       <c r="D65" s="4"/>
       <c r="E65" s="4"/>
@@ -3069,13 +2865,13 @@
     </row>
     <row r="66" spans="1:8" ht="15" customHeight="1">
       <c r="A66" s="18" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="B66" s="18">
         <v>3.9063000000000001E-2</v>
       </c>
       <c r="C66" s="18">
-        <v>6.4158999999999997</v>
+        <v>-4.4972149201203102</v>
       </c>
       <c r="D66" s="4"/>
       <c r="E66" s="4"/>
@@ -3085,13 +2881,13 @@
     </row>
     <row r="67" spans="1:8" ht="15" customHeight="1">
       <c r="A67" s="18" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="B67" s="18">
         <v>20</v>
       </c>
       <c r="C67" s="18">
-        <v>79</v>
+        <v>-4.1243850381579303</v>
       </c>
       <c r="D67" s="4"/>
       <c r="E67" s="4"/>
@@ -3101,13 +2897,13 @@
     </row>
     <row r="68" spans="1:8" ht="15" customHeight="1">
       <c r="A68" s="18" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="B68" s="18">
         <v>10</v>
       </c>
       <c r="C68" s="18">
-        <v>98.921999999999997</v>
+        <v>15.889552426524499</v>
       </c>
       <c r="D68" s="4"/>
       <c r="E68" s="4"/>
@@ -3117,13 +2913,13 @@
     </row>
     <row r="69" spans="1:8" ht="15" customHeight="1">
       <c r="A69" s="18" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="B69" s="18">
         <v>5</v>
       </c>
       <c r="C69" s="18">
-        <v>91.256</v>
+        <v>10.264658106025299</v>
       </c>
       <c r="D69" s="4"/>
       <c r="E69" s="4"/>
@@ -3133,13 +2929,13 @@
     </row>
     <row r="70" spans="1:8" ht="15" customHeight="1">
       <c r="A70" s="18" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="B70" s="18">
         <v>2.5</v>
       </c>
       <c r="C70" s="18">
-        <v>85.076999999999998</v>
+        <v>-1.4066517597529999</v>
       </c>
       <c r="D70" s="4"/>
       <c r="E70" s="4"/>
@@ -3149,13 +2945,13 @@
     </row>
     <row r="71" spans="1:8" ht="15" customHeight="1">
       <c r="A71" s="18" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="B71" s="18">
         <v>1.25</v>
       </c>
       <c r="C71" s="18">
-        <v>75.295000000000002</v>
+        <v>2.00639778515324</v>
       </c>
       <c r="D71" s="4"/>
       <c r="E71" s="4"/>
@@ -3165,13 +2961,13 @@
     </row>
     <row r="72" spans="1:8" ht="15" customHeight="1">
       <c r="A72" s="18" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="B72" s="18">
         <v>0.625</v>
       </c>
       <c r="C72" s="18">
-        <v>60.820999999999998</v>
+        <v>3.9991349959745999</v>
       </c>
       <c r="D72" s="4"/>
       <c r="E72" s="4"/>
@@ -3181,13 +2977,13 @@
     </row>
     <row r="73" spans="1:8" ht="15" customHeight="1">
       <c r="A73" s="18" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="B73" s="18">
         <v>0.3125</v>
       </c>
       <c r="C73" s="18">
-        <v>41.655999999999999</v>
+        <v>16.0822849534452</v>
       </c>
       <c r="D73" s="4"/>
       <c r="E73" s="4"/>
@@ -3197,13 +2993,13 @@
     </row>
     <row r="74" spans="1:8" ht="15" customHeight="1">
       <c r="A74" s="18" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="B74" s="18">
         <v>0.15625</v>
       </c>
       <c r="C74" s="18">
-        <v>36.965000000000003</v>
+        <v>-0.20011103013530401</v>
       </c>
       <c r="D74" s="4"/>
       <c r="E74" s="4"/>
@@ -3213,13 +3009,13 @@
     </row>
     <row r="75" spans="1:8" ht="15" customHeight="1">
       <c r="A75" s="18" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="B75" s="18">
         <v>7.8125E-2</v>
       </c>
       <c r="C75" s="18">
-        <v>25.295000000000002</v>
+        <v>-4.2483327689115002</v>
       </c>
       <c r="D75" s="4"/>
       <c r="E75" s="4"/>
@@ -3229,13 +3025,13 @@
     </row>
     <row r="76" spans="1:8" ht="15" customHeight="1">
       <c r="A76" s="18" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="B76" s="18">
         <v>3.9063000000000001E-2</v>
       </c>
       <c r="C76" s="18">
-        <v>18.085999999999999</v>
+        <v>17.123693372122901</v>
       </c>
       <c r="D76" s="4"/>
       <c r="E76" s="4"/>
@@ -3245,7 +3041,7 @@
     </row>
     <row r="77" spans="1:8" ht="15" customHeight="1">
       <c r="A77" s="18" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="B77" s="18">
         <v>0.3125</v>
@@ -3261,7 +3057,7 @@
     </row>
     <row r="78" spans="1:8" ht="15" customHeight="1">
       <c r="A78" s="18" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="B78" s="18">
         <v>0.15625</v>
@@ -3277,7 +3073,7 @@
     </row>
     <row r="79" spans="1:8" ht="15" customHeight="1">
       <c r="A79" s="18" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="B79" s="18">
         <v>7.8125E-2</v>
@@ -3293,7 +3089,7 @@
     </row>
     <row r="80" spans="1:8" ht="15" customHeight="1">
       <c r="A80" s="18" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="B80" s="18">
         <v>3.9063000000000001E-2</v>
@@ -3309,7 +3105,7 @@
     </row>
     <row r="81" spans="1:8" ht="15" customHeight="1">
       <c r="A81" s="18" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="B81" s="18">
         <v>20</v>
@@ -3325,7 +3121,7 @@
     </row>
     <row r="82" spans="1:8" ht="15" customHeight="1">
       <c r="A82" s="18" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="B82" s="18">
         <v>10</v>
@@ -3341,7 +3137,7 @@
     </row>
     <row r="83" spans="1:8" ht="15" customHeight="1">
       <c r="A83" s="18" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="B83" s="18">
         <v>5</v>
@@ -3357,7 +3153,7 @@
     </row>
     <row r="84" spans="1:8" ht="15" customHeight="1">
       <c r="A84" s="18" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="B84" s="18">
         <v>2.5</v>
@@ -3373,7 +3169,7 @@
     </row>
     <row r="85" spans="1:8" ht="15" customHeight="1">
       <c r="A85" s="18" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="B85" s="18">
         <v>1.25</v>
@@ -3389,7 +3185,7 @@
     </row>
     <row r="86" spans="1:8" ht="15" customHeight="1">
       <c r="A86" s="18" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="B86" s="18">
         <v>0.625</v>
@@ -3405,7 +3201,7 @@
     </row>
     <row r="87" spans="1:8" ht="15" customHeight="1">
       <c r="A87" s="18" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="B87" s="18">
         <v>0.3125</v>
@@ -3421,7 +3217,7 @@
     </row>
     <row r="88" spans="1:8" ht="15" customHeight="1">
       <c r="A88" s="18" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="B88" s="18">
         <v>0.15625</v>
@@ -3437,7 +3233,7 @@
     </row>
     <row r="89" spans="1:8" ht="15" customHeight="1">
       <c r="A89" s="18" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="B89" s="18">
         <v>7.8125E-2</v>
@@ -3453,7 +3249,7 @@
     </row>
     <row r="90" spans="1:8" ht="15" customHeight="1">
       <c r="A90" s="18" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="B90" s="18">
         <v>3.9063000000000001E-2</v>
@@ -3469,7 +3265,7 @@
     </row>
     <row r="91" spans="1:8" ht="15" customHeight="1">
       <c r="A91" s="18" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="B91" s="18">
         <v>20</v>
@@ -3485,7 +3281,7 @@
     </row>
     <row r="92" spans="1:8" ht="15" customHeight="1">
       <c r="A92" s="18" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="B92" s="18">
         <v>10</v>
@@ -3501,7 +3297,7 @@
     </row>
     <row r="93" spans="1:8" ht="15" customHeight="1">
       <c r="A93" s="18" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="B93" s="18">
         <v>5</v>
@@ -3517,7 +3313,7 @@
     </row>
     <row r="94" spans="1:8" ht="15" customHeight="1">
       <c r="A94" s="18" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="B94" s="18">
         <v>2.5</v>
@@ -3533,7 +3329,7 @@
     </row>
     <row r="95" spans="1:8" ht="15" customHeight="1">
       <c r="A95" s="18" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="B95" s="18">
         <v>1.25</v>
@@ -3549,7 +3345,7 @@
     </row>
     <row r="96" spans="1:8" ht="15" customHeight="1">
       <c r="A96" s="18" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="B96" s="18">
         <v>0.625</v>
@@ -3565,7 +3361,7 @@
     </row>
     <row r="97" spans="1:8" ht="15" customHeight="1">
       <c r="A97" s="18" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="B97" s="18">
         <v>0.3125</v>
@@ -3581,7 +3377,7 @@
     </row>
     <row r="98" spans="1:8" ht="15" customHeight="1">
       <c r="A98" s="18" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="B98" s="18">
         <v>0.15625</v>
@@ -3597,7 +3393,7 @@
     </row>
     <row r="99" spans="1:8" ht="15" customHeight="1">
       <c r="A99" s="18" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="B99" s="18">
         <v>7.8125E-2</v>
@@ -3613,7 +3409,7 @@
     </row>
     <row r="100" spans="1:8" ht="15" customHeight="1">
       <c r="A100" s="18" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="B100" s="18">
         <v>3.9063000000000001E-2</v>
@@ -3629,7 +3425,7 @@
     </row>
     <row r="101" spans="1:8" ht="15" customHeight="1">
       <c r="A101" s="18" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="B101" s="18">
         <v>20</v>
@@ -3645,7 +3441,7 @@
     </row>
     <row r="102" spans="1:8" ht="15" customHeight="1">
       <c r="A102" s="18" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="B102" s="18">
         <v>10</v>
@@ -3661,7 +3457,7 @@
     </row>
     <row r="103" spans="1:8" ht="15" customHeight="1">
       <c r="A103" s="18" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="B103" s="18">
         <v>5</v>
@@ -3677,7 +3473,7 @@
     </row>
     <row r="104" spans="1:8" ht="15" customHeight="1">
       <c r="A104" s="18" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="B104" s="18">
         <v>2.5</v>
@@ -3693,7 +3489,7 @@
     </row>
     <row r="105" spans="1:8" ht="15" customHeight="1">
       <c r="A105" s="18" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="B105" s="18">
         <v>1.25</v>
@@ -3709,7 +3505,7 @@
     </row>
     <row r="106" spans="1:8" ht="15" customHeight="1">
       <c r="A106" s="18" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="B106" s="18">
         <v>0.625</v>
@@ -3725,7 +3521,7 @@
     </row>
     <row r="107" spans="1:8" ht="15" customHeight="1">
       <c r="A107" s="18" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="B107" s="18">
         <v>0.3125</v>
@@ -3741,7 +3537,7 @@
     </row>
     <row r="108" spans="1:8" ht="15" customHeight="1">
       <c r="A108" s="18" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="B108" s="18">
         <v>0.15625</v>
@@ -3757,7 +3553,7 @@
     </row>
     <row r="109" spans="1:8" ht="15" customHeight="1">
       <c r="A109" s="18" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="B109" s="18">
         <v>7.8125E-2</v>
@@ -3773,7 +3569,7 @@
     </row>
     <row r="110" spans="1:8" ht="15" customHeight="1">
       <c r="A110" s="18" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="B110" s="18">
         <v>3.9063000000000001E-2</v>
@@ -3789,7 +3585,7 @@
     </row>
     <row r="111" spans="1:8" ht="15" customHeight="1">
       <c r="A111" s="18" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="B111" s="18">
         <v>20</v>
@@ -3805,7 +3601,7 @@
     </row>
     <row r="112" spans="1:8" ht="15" customHeight="1">
       <c r="A112" s="18" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="B112" s="18">
         <v>10</v>
@@ -3821,7 +3617,7 @@
     </row>
     <row r="113" spans="1:8" ht="15" customHeight="1">
       <c r="A113" s="18" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="B113" s="18">
         <v>5</v>
@@ -3837,7 +3633,7 @@
     </row>
     <row r="114" spans="1:8" ht="15" customHeight="1">
       <c r="A114" s="18" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="B114" s="18">
         <v>2.5</v>
@@ -3853,7 +3649,7 @@
     </row>
     <row r="115" spans="1:8" ht="15" customHeight="1">
       <c r="A115" s="18" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="B115" s="18">
         <v>1.25</v>
@@ -3869,7 +3665,7 @@
     </row>
     <row r="116" spans="1:8" ht="15" customHeight="1">
       <c r="A116" s="18" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="B116" s="18">
         <v>0.625</v>
@@ -3885,7 +3681,7 @@
     </row>
     <row r="117" spans="1:8" ht="15" customHeight="1">
       <c r="A117" s="18" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="B117" s="18">
         <v>20</v>
@@ -3901,7 +3697,7 @@
     </row>
     <row r="118" spans="1:8" ht="15" customHeight="1">
       <c r="A118" s="18" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="B118" s="18">
         <v>10</v>
@@ -3917,7 +3713,7 @@
     </row>
     <row r="119" spans="1:8" ht="15" customHeight="1">
       <c r="A119" s="18" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="B119" s="18">
         <v>5</v>
@@ -3933,7 +3729,7 @@
     </row>
     <row r="120" spans="1:8" ht="15" customHeight="1">
       <c r="A120" s="18" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="B120" s="18">
         <v>2.5</v>
@@ -3949,7 +3745,7 @@
     </row>
     <row r="121" spans="1:8" ht="15" customHeight="1">
       <c r="A121" s="18" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="B121" s="18">
         <v>1.25</v>
@@ -3965,7 +3761,7 @@
     </row>
     <row r="122" spans="1:8" ht="15" customHeight="1">
       <c r="A122" s="18" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="B122" s="18">
         <v>0.625</v>
@@ -3981,7 +3777,7 @@
     </row>
     <row r="123" spans="1:8" ht="15" customHeight="1">
       <c r="A123" s="18" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="B123" s="18">
         <v>0.3125</v>
@@ -3997,7 +3793,7 @@
     </row>
     <row r="124" spans="1:8" ht="15" customHeight="1">
       <c r="A124" s="18" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="B124" s="18">
         <v>0.15625</v>
@@ -4013,7 +3809,7 @@
     </row>
     <row r="125" spans="1:8" ht="15" customHeight="1">
       <c r="A125" s="18" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="B125" s="18">
         <v>7.8125E-2</v>
@@ -4029,7 +3825,7 @@
     </row>
     <row r="126" spans="1:8" ht="15" customHeight="1">
       <c r="A126" s="18" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="B126" s="18">
         <v>3.9063000000000001E-2</v>
@@ -4045,7 +3841,7 @@
     </row>
     <row r="127" spans="1:8" ht="15" customHeight="1">
       <c r="A127" s="18" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="B127" s="18">
         <v>20</v>
@@ -4061,7 +3857,7 @@
     </row>
     <row r="128" spans="1:8" ht="15" customHeight="1">
       <c r="A128" s="18" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="B128" s="18">
         <v>10</v>
@@ -4077,7 +3873,7 @@
     </row>
     <row r="129" spans="1:8" ht="15" customHeight="1">
       <c r="A129" s="18" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="B129" s="18">
         <v>5</v>
@@ -4093,7 +3889,7 @@
     </row>
     <row r="130" spans="1:8" ht="15" customHeight="1">
       <c r="A130" s="18" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="B130" s="18">
         <v>2.5</v>
@@ -4109,7 +3905,7 @@
     </row>
     <row r="131" spans="1:8" ht="15" customHeight="1">
       <c r="A131" s="18" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="B131" s="18">
         <v>1.25</v>
@@ -4125,7 +3921,7 @@
     </row>
     <row r="132" spans="1:8" ht="15" customHeight="1">
       <c r="A132" s="18" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="B132" s="18">
         <v>0.625</v>
@@ -4141,7 +3937,7 @@
     </row>
     <row r="133" spans="1:8" ht="15" customHeight="1">
       <c r="A133" s="18" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="B133" s="18">
         <v>0.3125</v>
@@ -4157,7 +3953,7 @@
     </row>
     <row r="134" spans="1:8" ht="15" customHeight="1">
       <c r="A134" s="18" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="B134" s="18">
         <v>0.15625</v>
@@ -4173,7 +3969,7 @@
     </row>
     <row r="135" spans="1:8" ht="15" customHeight="1">
       <c r="A135" s="18" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="B135" s="18">
         <v>7.8125E-2</v>
@@ -4189,7 +3985,7 @@
     </row>
     <row r="136" spans="1:8" ht="15" customHeight="1">
       <c r="A136" s="18" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="B136" s="18">
         <v>3.9063000000000001E-2</v>
@@ -4205,7 +4001,7 @@
     </row>
     <row r="137" spans="1:8" ht="15" customHeight="1">
       <c r="A137" s="18" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="B137" s="18">
         <v>20</v>
@@ -4221,7 +4017,7 @@
     </row>
     <row r="138" spans="1:8" ht="15" customHeight="1">
       <c r="A138" s="18" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="B138" s="18">
         <v>10</v>
@@ -4237,7 +4033,7 @@
     </row>
     <row r="139" spans="1:8" ht="15" customHeight="1">
       <c r="A139" s="18" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="B139" s="18">
         <v>5</v>
@@ -4253,7 +4049,7 @@
     </row>
     <row r="140" spans="1:8" ht="15" customHeight="1">
       <c r="A140" s="18" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="B140" s="18">
         <v>2.5</v>
@@ -4269,7 +4065,7 @@
     </row>
     <row r="141" spans="1:8" ht="15" customHeight="1">
       <c r="A141" s="18" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="B141" s="18">
         <v>1.25</v>
@@ -4285,7 +4081,7 @@
     </row>
     <row r="142" spans="1:8" ht="15" customHeight="1">
       <c r="A142" s="18" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="B142" s="18">
         <v>0.625</v>
@@ -4301,7 +4097,7 @@
     </row>
     <row r="143" spans="1:8" ht="15" customHeight="1">
       <c r="A143" s="18" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="B143" s="18">
         <v>0.3125</v>
@@ -4317,7 +4113,7 @@
     </row>
     <row r="144" spans="1:8" ht="15" customHeight="1">
       <c r="A144" s="18" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="B144" s="18">
         <v>0.15625</v>
@@ -4333,7 +4129,7 @@
     </row>
     <row r="145" spans="1:8" ht="15" customHeight="1">
       <c r="A145" s="18" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="B145" s="18">
         <v>7.8125E-2</v>
@@ -4349,7 +4145,7 @@
     </row>
     <row r="146" spans="1:8" ht="15" customHeight="1">
       <c r="A146" s="18" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="B146" s="18">
         <v>3.9063000000000001E-2</v>
@@ -4365,7 +4161,7 @@
     </row>
     <row r="147" spans="1:8" ht="15" customHeight="1">
       <c r="A147" s="18" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="B147" s="18">
         <v>20</v>
@@ -4381,7 +4177,7 @@
     </row>
     <row r="148" spans="1:8" ht="15" customHeight="1">
       <c r="A148" s="18" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="B148" s="18">
         <v>10</v>
@@ -4397,7 +4193,7 @@
     </row>
     <row r="149" spans="1:8" ht="15" customHeight="1">
       <c r="A149" s="18" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="B149" s="18">
         <v>5</v>
@@ -4413,7 +4209,7 @@
     </row>
     <row r="150" spans="1:8" ht="15" customHeight="1">
       <c r="A150" s="18" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="B150" s="18">
         <v>2.5</v>
@@ -4429,7 +4225,7 @@
     </row>
     <row r="151" spans="1:8" ht="15" customHeight="1">
       <c r="A151" s="18" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="B151" s="18">
         <v>1.25</v>
@@ -4445,7 +4241,7 @@
     </row>
     <row r="152" spans="1:8" ht="15" customHeight="1">
       <c r="A152" s="18" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="B152" s="18">
         <v>0.625</v>
@@ -4461,7 +4257,7 @@
     </row>
     <row r="153" spans="1:8" ht="15" customHeight="1">
       <c r="A153" s="18" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="B153" s="18">
         <v>0.3125</v>
@@ -4477,7 +4273,7 @@
     </row>
     <row r="154" spans="1:8" ht="15" customHeight="1">
       <c r="A154" s="18" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="B154" s="18">
         <v>0.15625</v>
@@ -4493,7 +4289,7 @@
     </row>
     <row r="155" spans="1:8" ht="15" customHeight="1">
       <c r="A155" s="18" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="B155" s="18">
         <v>7.8125E-2</v>
@@ -4509,7 +4305,7 @@
     </row>
     <row r="156" spans="1:8" ht="15" customHeight="1">
       <c r="A156" s="18" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="B156" s="18">
         <v>3.9063000000000001E-2</v>
@@ -4525,7 +4321,7 @@
     </row>
     <row r="157" spans="1:8" ht="15" customHeight="1">
       <c r="A157" s="18" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="B157" s="18">
         <v>20</v>
@@ -4541,7 +4337,7 @@
     </row>
     <row r="158" spans="1:8" ht="15" customHeight="1">
       <c r="A158" s="18" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="B158" s="18">
         <v>10</v>
@@ -4557,7 +4353,7 @@
     </row>
     <row r="159" spans="1:8" ht="15" customHeight="1">
       <c r="A159" s="18" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="B159" s="18">
         <v>5</v>
@@ -4573,7 +4369,7 @@
     </row>
     <row r="160" spans="1:8" ht="15" customHeight="1">
       <c r="A160" s="18" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="B160" s="18">
         <v>2.5</v>
@@ -4589,7 +4385,7 @@
     </row>
     <row r="161" spans="1:8" ht="15" customHeight="1">
       <c r="A161" s="18" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="B161" s="18">
         <v>1.25</v>
@@ -4605,7 +4401,7 @@
     </row>
     <row r="162" spans="1:8" ht="15" customHeight="1">
       <c r="A162" s="18" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="B162" s="18">
         <v>0.625</v>
@@ -4621,7 +4417,7 @@
     </row>
     <row r="163" spans="1:8" ht="15" customHeight="1">
       <c r="A163" s="18" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="B163" s="18">
         <v>0.3125</v>
@@ -4637,7 +4433,7 @@
     </row>
     <row r="164" spans="1:8" ht="15" customHeight="1">
       <c r="A164" s="18" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="B164" s="18">
         <v>0.15625</v>
@@ -4653,7 +4449,7 @@
     </row>
     <row r="165" spans="1:8" ht="15" customHeight="1">
       <c r="A165" s="18" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="B165" s="18">
         <v>7.8125E-2</v>
@@ -4669,7 +4465,7 @@
     </row>
     <row r="166" spans="1:8" ht="15" customHeight="1">
       <c r="A166" s="18" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="B166" s="18">
         <v>3.9063000000000001E-2</v>
@@ -4685,7 +4481,7 @@
     </row>
     <row r="167" spans="1:8" ht="15" customHeight="1">
       <c r="A167" s="18" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="B167" s="18">
         <v>20</v>
@@ -4701,7 +4497,7 @@
     </row>
     <row r="168" spans="1:8" ht="15" customHeight="1">
       <c r="A168" s="18" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="B168" s="18">
         <v>10</v>
@@ -4717,7 +4513,7 @@
     </row>
     <row r="169" spans="1:8" ht="15" customHeight="1">
       <c r="A169" s="18" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="B169" s="18">
         <v>5</v>
@@ -4733,7 +4529,7 @@
     </row>
     <row r="170" spans="1:8" ht="15" customHeight="1">
       <c r="A170" s="18" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="B170" s="18">
         <v>2.5</v>
@@ -4749,7 +4545,7 @@
     </row>
     <row r="171" spans="1:8" ht="15" customHeight="1">
       <c r="A171" s="18" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="B171" s="18">
         <v>1.25</v>
@@ -4765,7 +4561,7 @@
     </row>
     <row r="172" spans="1:8" ht="15" customHeight="1">
       <c r="A172" s="18" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="B172" s="18">
         <v>0.625</v>
@@ -4781,7 +4577,7 @@
     </row>
     <row r="173" spans="1:8" ht="15" customHeight="1">
       <c r="A173" s="18" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="B173" s="18">
         <v>0.3125</v>
@@ -4797,7 +4593,7 @@
     </row>
     <row r="174" spans="1:8" ht="15" customHeight="1">
       <c r="A174" s="18" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="B174" s="18">
         <v>0.15625</v>
@@ -4813,7 +4609,7 @@
     </row>
     <row r="175" spans="1:8" ht="15" customHeight="1">
       <c r="A175" s="18" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="B175" s="18">
         <v>7.8125E-2</v>
@@ -4829,7 +4625,7 @@
     </row>
     <row r="176" spans="1:8" ht="15" customHeight="1">
       <c r="A176" s="18" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="B176" s="18">
         <v>3.9063000000000001E-2</v>
@@ -4845,7 +4641,7 @@
     </row>
     <row r="177" spans="1:8" ht="15" customHeight="1">
       <c r="A177" s="18" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="B177" s="18">
         <v>20</v>
@@ -4861,7 +4657,7 @@
     </row>
     <row r="178" spans="1:8" ht="15" customHeight="1">
       <c r="A178" s="18" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="B178" s="18">
         <v>10</v>
@@ -4877,7 +4673,7 @@
     </row>
     <row r="179" spans="1:8" ht="15" customHeight="1">
       <c r="A179" s="18" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="B179" s="18">
         <v>5</v>
@@ -4893,7 +4689,7 @@
     </row>
     <row r="180" spans="1:8" ht="15" customHeight="1">
       <c r="A180" s="18" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="B180" s="18">
         <v>2.5</v>
@@ -4909,7 +4705,7 @@
     </row>
     <row r="181" spans="1:8" ht="15" customHeight="1">
       <c r="A181" s="18" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="B181" s="18">
         <v>1.25</v>
@@ -4925,7 +4721,7 @@
     </row>
     <row r="182" spans="1:8" ht="15" customHeight="1">
       <c r="A182" s="18" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="B182" s="18">
         <v>0.625</v>
@@ -4941,7 +4737,7 @@
     </row>
     <row r="183" spans="1:8" ht="15" customHeight="1">
       <c r="A183" s="18" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="B183" s="18">
         <v>0.3125</v>
@@ -4957,7 +4753,7 @@
     </row>
     <row r="184" spans="1:8" ht="15" customHeight="1">
       <c r="A184" s="18" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="B184" s="18">
         <v>0.15625</v>
@@ -4973,7 +4769,7 @@
     </row>
     <row r="185" spans="1:8" ht="15" customHeight="1">
       <c r="A185" s="18" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="B185" s="18">
         <v>7.8125E-2</v>
@@ -4989,7 +4785,7 @@
     </row>
     <row r="186" spans="1:8" ht="15" customHeight="1">
       <c r="A186" s="18" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="B186" s="18">
         <v>3.9063000000000001E-2</v>
@@ -5005,7 +4801,7 @@
     </row>
     <row r="187" spans="1:8" ht="15" customHeight="1">
       <c r="A187" s="18" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="B187" s="18">
         <v>20</v>
@@ -5021,7 +4817,7 @@
     </row>
     <row r="188" spans="1:8" ht="15" customHeight="1">
       <c r="A188" s="18" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="B188" s="18">
         <v>10</v>
@@ -5037,7 +4833,7 @@
     </row>
     <row r="189" spans="1:8" ht="15" customHeight="1">
       <c r="A189" s="18" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="B189" s="18">
         <v>5</v>
@@ -5053,7 +4849,7 @@
     </row>
     <row r="190" spans="1:8" ht="15" customHeight="1">
       <c r="A190" s="18" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="B190" s="18">
         <v>2.5</v>
@@ -5069,7 +4865,7 @@
     </row>
     <row r="191" spans="1:8" ht="15" customHeight="1">
       <c r="A191" s="18" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="B191" s="18">
         <v>1.25</v>
@@ -5085,7 +4881,7 @@
     </row>
     <row r="192" spans="1:8" ht="15" customHeight="1">
       <c r="A192" s="18" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="B192" s="18">
         <v>0.625</v>
@@ -5101,7 +4897,7 @@
     </row>
     <row r="193" spans="1:8" ht="15" customHeight="1">
       <c r="A193" s="18" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="B193" s="18">
         <v>0.3125</v>
@@ -5117,7 +4913,7 @@
     </row>
     <row r="194" spans="1:8" ht="15" customHeight="1">
       <c r="A194" s="18" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="B194" s="18">
         <v>0.15625</v>
@@ -5133,7 +4929,7 @@
     </row>
     <row r="195" spans="1:8" ht="15" customHeight="1">
       <c r="A195" s="18" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="B195" s="18">
         <v>20</v>
@@ -5149,7 +4945,7 @@
     </row>
     <row r="196" spans="1:8" ht="15" customHeight="1">
       <c r="A196" s="18" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="B196" s="18">
         <v>10</v>
@@ -5165,7 +4961,7 @@
     </row>
     <row r="197" spans="1:8" ht="15" customHeight="1">
       <c r="A197" s="18" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="B197" s="18">
         <v>5</v>
@@ -5181,7 +4977,7 @@
     </row>
     <row r="198" spans="1:8" ht="15" customHeight="1">
       <c r="A198" s="18" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="B198" s="18">
         <v>2.5</v>
@@ -5197,7 +4993,7 @@
     </row>
     <row r="199" spans="1:8" ht="15" customHeight="1">
       <c r="A199" s="18" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="B199" s="18">
         <v>1.25</v>
@@ -5213,7 +5009,7 @@
     </row>
     <row r="200" spans="1:8" ht="15" customHeight="1">
       <c r="A200" s="18" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="B200" s="18">
         <v>0.625</v>
@@ -5229,7 +5025,7 @@
     </row>
     <row r="201" spans="1:8" ht="15" customHeight="1">
       <c r="A201" s="18" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="B201" s="18">
         <v>0.3125</v>
@@ -5245,7 +5041,7 @@
     </row>
     <row r="202" spans="1:8" ht="15" customHeight="1">
       <c r="A202" s="18" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="B202" s="18">
         <v>0.15625</v>
@@ -5261,7 +5057,7 @@
     </row>
     <row r="203" spans="1:8" ht="15" customHeight="1">
       <c r="A203" s="18" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="B203" s="18">
         <v>7.8125E-2</v>
@@ -5277,7 +5073,7 @@
     </row>
     <row r="204" spans="1:8" ht="15" customHeight="1">
       <c r="A204" s="18" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="B204" s="18">
         <v>3.9063000000000001E-2</v>
@@ -5293,7 +5089,7 @@
     </row>
     <row r="205" spans="1:8" ht="15" customHeight="1">
       <c r="A205" s="18" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="B205" s="18">
         <v>7.8125E-2</v>
@@ -5309,7 +5105,7 @@
     </row>
     <row r="206" spans="1:8" ht="15" customHeight="1">
       <c r="A206" s="18" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="B206" s="18">
         <v>3.9063000000000001E-2</v>
@@ -5325,7 +5121,7 @@
     </row>
     <row r="207" spans="1:8" ht="15" customHeight="1">
       <c r="A207" s="18" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="B207" s="18">
         <v>20</v>
@@ -5341,7 +5137,7 @@
     </row>
     <row r="208" spans="1:8" ht="15" customHeight="1">
       <c r="A208" s="18" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="B208" s="18">
         <v>10</v>
@@ -5357,7 +5153,7 @@
     </row>
     <row r="209" spans="1:8" ht="15" customHeight="1">
       <c r="A209" s="18" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="B209" s="18">
         <v>5</v>
@@ -5373,7 +5169,7 @@
     </row>
     <row r="210" spans="1:8" ht="15" customHeight="1">
       <c r="A210" s="18" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="B210" s="18">
         <v>2.5</v>
@@ -5389,7 +5185,7 @@
     </row>
     <row r="211" spans="1:8" ht="15" customHeight="1">
       <c r="A211" s="18" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="B211" s="18">
         <v>1.25</v>
@@ -5405,7 +5201,7 @@
     </row>
     <row r="212" spans="1:8" ht="15" customHeight="1">
       <c r="A212" s="18" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="B212" s="18">
         <v>0.625</v>
@@ -5421,7 +5217,7 @@
     </row>
     <row r="213" spans="1:8" ht="15" customHeight="1">
       <c r="A213" s="18" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="B213" s="18">
         <v>0.3125</v>
@@ -5437,7 +5233,7 @@
     </row>
     <row r="214" spans="1:8" ht="15" customHeight="1">
       <c r="A214" s="18" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="B214" s="18">
         <v>0.15625</v>
@@ -5453,7 +5249,7 @@
     </row>
     <row r="215" spans="1:8" ht="15" customHeight="1">
       <c r="A215" s="18" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="B215" s="18">
         <v>7.8125E-2</v>
@@ -5469,7 +5265,7 @@
     </row>
     <row r="216" spans="1:8" ht="15" customHeight="1">
       <c r="A216" s="18" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="B216" s="18">
         <v>3.9063000000000001E-2</v>
@@ -5485,7 +5281,7 @@
     </row>
     <row r="217" spans="1:8" ht="15" customHeight="1">
       <c r="A217" s="18" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="B217" s="18">
         <v>20</v>
@@ -5501,7 +5297,7 @@
     </row>
     <row r="218" spans="1:8" ht="15" customHeight="1">
       <c r="A218" s="18" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="B218" s="18">
         <v>10</v>
@@ -5517,7 +5313,7 @@
     </row>
     <row r="219" spans="1:8" ht="15" customHeight="1">
       <c r="A219" s="18" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="B219" s="18">
         <v>5</v>
@@ -5533,7 +5329,7 @@
     </row>
     <row r="220" spans="1:8" ht="15" customHeight="1">
       <c r="A220" s="18" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="B220" s="18">
         <v>2.5</v>
@@ -5549,7 +5345,7 @@
     </row>
     <row r="221" spans="1:8" ht="15" customHeight="1">
       <c r="A221" s="18" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="B221" s="18">
         <v>1.25</v>
@@ -5565,7 +5361,7 @@
     </row>
     <row r="222" spans="1:8" ht="15" customHeight="1">
       <c r="A222" s="18" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="B222" s="18">
         <v>0.625</v>
@@ -5581,7 +5377,7 @@
     </row>
     <row r="223" spans="1:8" ht="15" customHeight="1">
       <c r="A223" s="18" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="B223" s="18">
         <v>0.3125</v>
@@ -5597,7 +5393,7 @@
     </row>
     <row r="224" spans="1:8" ht="15" customHeight="1">
       <c r="A224" s="18" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="B224" s="18">
         <v>0.15625</v>
@@ -5613,7 +5409,7 @@
     </row>
     <row r="225" spans="1:8" ht="15" customHeight="1">
       <c r="A225" s="18" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="B225" s="18">
         <v>7.8125E-2</v>
@@ -5629,7 +5425,7 @@
     </row>
     <row r="226" spans="1:8" ht="15" customHeight="1">
       <c r="A226" s="18" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="B226" s="18">
         <v>3.9063000000000001E-2</v>
@@ -5645,7 +5441,7 @@
     </row>
     <row r="227" spans="1:8" ht="15" customHeight="1">
       <c r="A227" s="18" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="B227" s="18">
         <v>20</v>
@@ -5661,7 +5457,7 @@
     </row>
     <row r="228" spans="1:8" ht="15" customHeight="1">
       <c r="A228" s="18" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="B228" s="18">
         <v>10</v>
@@ -5677,7 +5473,7 @@
     </row>
     <row r="229" spans="1:8" ht="15" customHeight="1">
       <c r="A229" s="18" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="B229" s="18">
         <v>5</v>
@@ -5693,7 +5489,7 @@
     </row>
     <row r="230" spans="1:8" ht="15" customHeight="1">
       <c r="A230" s="18" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="B230" s="18">
         <v>2.5</v>
@@ -5709,7 +5505,7 @@
     </row>
     <row r="231" spans="1:8" ht="15" customHeight="1">
       <c r="A231" s="18" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="B231" s="18">
         <v>1.25</v>
@@ -5725,7 +5521,7 @@
     </row>
     <row r="232" spans="1:8" ht="15" customHeight="1">
       <c r="A232" s="18" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="B232" s="18">
         <v>0.625</v>
@@ -5741,7 +5537,7 @@
     </row>
     <row r="233" spans="1:8" ht="15" customHeight="1">
       <c r="A233" s="18" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="B233" s="18">
         <v>0.3125</v>
@@ -5757,7 +5553,7 @@
     </row>
     <row r="234" spans="1:8" ht="15" customHeight="1">
       <c r="A234" s="18" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="B234" s="18">
         <v>0.15625</v>
@@ -5773,7 +5569,7 @@
     </row>
     <row r="235" spans="1:8" ht="15" customHeight="1">
       <c r="A235" s="18" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="B235" s="18">
         <v>7.8125E-2</v>
@@ -5789,7 +5585,7 @@
     </row>
     <row r="236" spans="1:8" ht="15" customHeight="1">
       <c r="A236" s="18" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="B236" s="18">
         <v>3.9063000000000001E-2</v>
@@ -7222,7 +7018,7 @@
         <v>-15.846</v>
       </c>
       <c r="D325" s="18" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="E325" s="4"/>
       <c r="F325" s="4"/>

</xml_diff>